<commit_message>
CCDC data files updates
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC03_CDSValidation_by_ParticipantID - 7.xlsx
+++ b/InputFiles/CDS/TC03_CDSValidation_by_ParticipantID - 7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\CDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9E5B09-6EBD-4A23-92DE-79F7C72DDD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1F0336-0F8D-4723-8C82-3EEE4C37A282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>dbExcel</t>
-  </si>
-  <si>
-    <t>WebExcel</t>
   </si>
   <si>
     <t>SamplesTab</t>
@@ -99,7 +96,10 @@
     <t>TC03_CDSValidation_by_ParticipantID - 7_Neo4jData.xlsx</t>
   </si>
   <si>
-    <t>TC03_CDSValidation_by_ParticipantID - 7_WebData.xlsx</t>
+    <t>ExDataExcel</t>
+  </si>
+  <si>
+    <t>TC03_CDSValidation_by_ParticipantID - 7_ExcelData.xlsx</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -445,18 +445,18 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="274.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -464,13 +464,13 @@
     </row>
     <row r="3" spans="1:4" ht="174" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -478,13 +478,13 @@
     </row>
     <row r="4" spans="1:4" ht="174" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>

</xml_diff>